<commit_message>
Add adruino code for testing with physical pedal
</commit_message>
<xml_diff>
--- a/arduino/CAN Bus/CAN Bus Messages.xlsx
+++ b/arduino/CAN Bus/CAN Bus Messages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/ev_club_sutd_edu_sg/Documents/EVC - Current Projects/EVAM/Motor, Controller, Battery/Sensors and Telemetry/CAN Bus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/CAN Bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="687" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2344DB95-3184-4735-B027-1DF51AF49817}"/>
+  <xr:revisionPtr revIDLastSave="689" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE08F356-55A9-42A0-9D37-B0EB1457C0A3}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1534" yWindow="-103" windowWidth="42455" windowHeight="24892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="175">
   <si>
     <t>Message ID (Decimal)</t>
   </si>
@@ -510,9 +510,6 @@
   </si>
   <si>
     <t>angle = (B1*256 + B2)/10 - 180; 0-360</t>
-  </si>
-  <si>
-    <t>0 =  ok, 1 = small error, 255 = fatal error</t>
   </si>
   <si>
     <t>for ECU and HUD to know that they are still connected</t>
@@ -564,6 +561,18 @@
   </si>
   <si>
     <t>FLW Status</t>
+  </si>
+  <si>
+    <t>0 =  error, 1 = ok, 255 = offline</t>
+  </si>
+  <si>
+    <t>1 =  error, 1 = ok, 255 = offline</t>
+  </si>
+  <si>
+    <t>2 =  error, 1 = ok, 255 = offline</t>
+  </si>
+  <si>
+    <t>3 =  error, 1 = ok, 255 = offline</t>
   </si>
 </sst>
 </file>
@@ -738,18 +747,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -758,6 +755,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -1060,23 +1069,23 @@
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="30" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="1.5703125" style="11" customWidth="1"/>
-    <col min="16" max="23" width="20.5703125" customWidth="1"/>
-    <col min="28" max="28" width="100.140625" style="5" customWidth="1"/>
-    <col min="29" max="29" width="2.5703125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="9.84375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="6.3046875" customWidth="1"/>
+    <col min="14" max="14" width="8.69140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="1.53515625" style="11" customWidth="1"/>
+    <col min="16" max="23" width="20.53515625" customWidth="1"/>
+    <col min="28" max="28" width="100.15234375" style="5" customWidth="1"/>
+    <col min="29" max="29" width="2.53515625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1086,23 +1095,23 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
       <c r="N1" s="9" t="s">
         <v>73</v>
       </c>
       <c r="O1" s="10"/>
       <c r="P1" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>102</v>
@@ -1136,7 +1145,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -1150,7 +1159,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B3">
         <v>1</v>
       </c>
@@ -1161,7 +1170,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B4">
         <v>2</v>
       </c>
@@ -1169,7 +1178,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B5">
         <v>3</v>
       </c>
@@ -1177,12 +1186,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>67</v>
@@ -1200,153 +1209,153 @@
         <v>74</v>
       </c>
       <c r="P6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AB6" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="23">
+    <row r="7" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="19">
         <v>5</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="AB7" s="28" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB7" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="AC7" s="27"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC7" s="23"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="23">
+    <row r="10" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="19">
         <v>8</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="M10" s="23" t="s">
+      <c r="M10" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="N10" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="O10" s="25"/>
-      <c r="P10" s="23" t="s">
+      <c r="N10" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="O10" s="21"/>
+      <c r="P10" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB10" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="AB10" s="26" t="s">
+      <c r="AC10" s="23"/>
+    </row>
+    <row r="11" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="19">
+        <v>9</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="O11" s="21"/>
+      <c r="P11" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB11" s="24"/>
+      <c r="AC11" s="23"/>
+    </row>
+    <row r="12" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="19">
+        <v>10</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="AC10" s="27"/>
-    </row>
-    <row r="11" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="23">
+      <c r="D12" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="M12" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="N12" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="O12" s="21"/>
+      <c r="P12" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="AB12" s="24"/>
+      <c r="AC12" s="23"/>
+    </row>
+    <row r="13" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="19">
+        <v>11</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="23" t="s">
+      <c r="E13" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="M11" s="23" t="s">
+      <c r="M13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="N11" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="O11" s="25"/>
-      <c r="P11" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB11" s="28"/>
-      <c r="AC11" s="27"/>
-    </row>
-    <row r="12" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="23">
-        <v>10</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="M12" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="N12" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="O12" s="25"/>
-      <c r="P12" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB12" s="28"/>
-      <c r="AC12" s="27"/>
-    </row>
-    <row r="13" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="23">
-        <v>11</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="M13" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="N13" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="O13" s="25"/>
-      <c r="P13" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB13" s="28"/>
-      <c r="AC13" s="27"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="N13" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="O13" s="21"/>
+      <c r="P13" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB13" s="24"/>
+      <c r="AC13" s="23"/>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B14">
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B15">
         <v>13</v>
       </c>
@@ -1354,7 +1363,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B16">
         <v>14</v>
       </c>
@@ -1362,7 +1371,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B17">
         <v>15</v>
       </c>
@@ -1370,82 +1379,82 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B32">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B33">
         <v>31</v>
       </c>
@@ -1453,7 +1462,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>82</v>
       </c>
@@ -1482,14 +1491,14 @@
         <v>119</v>
       </c>
       <c r="T34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Y34">
         <v>51</v>
       </c>
       <c r="AB34" s="6"/>
     </row>
-    <row r="35" spans="1:30" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" s="12" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="B35" s="12">
         <v>33</v>
       </c>
@@ -1526,7 +1535,7 @@
       </c>
       <c r="AC35" s="16"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B36">
         <v>34</v>
       </c>
@@ -1534,12 +1543,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B37">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B38">
         <v>36</v>
       </c>
@@ -1558,18 +1567,18 @@
       <c r="N38" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="P38" s="20" t="s">
+      <c r="P38" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="Q38" s="20"/>
-      <c r="R38" s="20" t="s">
+      <c r="Q38" s="26"/>
+      <c r="R38" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="S38" s="20"/>
-      <c r="T38" s="20" t="s">
+      <c r="S38" s="26"/>
+      <c r="T38" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="U38" s="20"/>
+      <c r="U38" s="26"/>
       <c r="V38" t="s">
         <v>120</v>
       </c>
@@ -1578,44 +1587,44 @@
       </c>
       <c r="AB38" s="6"/>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B39">
         <v>37</v>
       </c>
       <c r="AB39" s="6"/>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B40">
         <v>38</v>
       </c>
       <c r="AB40" s="6"/>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B41">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B42">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B43">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B44">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B45">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B46">
         <v>44</v>
       </c>
@@ -1642,22 +1651,22 @@
       </c>
       <c r="AB46" s="6"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B47">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.4">
       <c r="B48">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B49">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B50">
         <v>48</v>
       </c>
@@ -1695,7 +1704,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B51" s="12">
         <v>49</v>
       </c>
@@ -1716,7 +1725,7 @@
       <c r="AB51" s="17"/>
       <c r="AC51" s="16"/>
     </row>
-    <row r="52" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B52" s="12">
         <v>50</v>
       </c>
@@ -1737,7 +1746,7 @@
       <c r="AB52" s="17"/>
       <c r="AC52" s="16"/>
     </row>
-    <row r="53" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B53" s="12">
         <v>51</v>
       </c>
@@ -1758,7 +1767,7 @@
       <c r="AB53" s="17"/>
       <c r="AC53" s="16"/>
     </row>
-    <row r="54" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B54">
         <v>52</v>
       </c>
@@ -1774,12 +1783,12 @@
       <c r="N54" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="P54" s="20" t="s">
+      <c r="P54" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="Q54" s="20"/>
-    </row>
-    <row r="55" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Q54" s="26"/>
+    </row>
+    <row r="55" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B55">
         <v>53</v>
       </c>
@@ -1792,12 +1801,12 @@
       <c r="E55" t="s">
         <v>4</v>
       </c>
-      <c r="P55" s="20" t="s">
+      <c r="P55" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="Q55" s="20"/>
-    </row>
-    <row r="56" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Q55" s="26"/>
+    </row>
+    <row r="56" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B56">
         <v>54</v>
       </c>
@@ -1810,12 +1819,12 @@
       <c r="E56" t="s">
         <v>4</v>
       </c>
-      <c r="P56" s="20" t="s">
+      <c r="P56" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="Q56" s="20"/>
-    </row>
-    <row r="57" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Q56" s="26"/>
+    </row>
+    <row r="57" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B57">
         <v>55</v>
       </c>
@@ -1828,12 +1837,12 @@
       <c r="E57" t="s">
         <v>4</v>
       </c>
-      <c r="P57" s="20" t="s">
+      <c r="P57" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="Q57" s="20"/>
-    </row>
-    <row r="58" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Q57" s="26"/>
+    </row>
+    <row r="58" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B58">
         <v>56</v>
       </c>
@@ -1849,47 +1858,47 @@
       <c r="N58" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="P58" s="20" t="s">
+      <c r="P58" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="Q58" s="20"/>
-    </row>
-    <row r="59" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="Q58" s="26"/>
+    </row>
+    <row r="59" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B59">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B60">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B61">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B62">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B63">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="2:29" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:29" x14ac:dyDescent="0.4">
       <c r="B64">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B65">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" s="12" t="s">
         <v>99</v>
       </c>
@@ -1929,7 +1938,7 @@
       </c>
       <c r="AC66" s="16"/>
     </row>
-    <row r="67" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B67" s="12">
         <v>65</v>
       </c>
@@ -1941,24 +1950,24 @@
       </c>
       <c r="N67" s="13"/>
       <c r="O67" s="14"/>
-      <c r="P67" s="21" t="s">
+      <c r="P67" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="Q67" s="21"/>
-      <c r="R67" s="21" t="s">
+      <c r="Q67" s="25"/>
+      <c r="R67" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="S67" s="21"/>
-      <c r="T67" s="21" t="s">
+      <c r="S67" s="25"/>
+      <c r="T67" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="U67" s="21"/>
+      <c r="U67" s="25"/>
       <c r="AB67" s="17" t="s">
         <v>153</v>
       </c>
       <c r="AC67" s="16"/>
     </row>
-    <row r="68" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B68" s="12">
         <v>66</v>
       </c>
@@ -1970,22 +1979,22 @@
       </c>
       <c r="N68" s="13"/>
       <c r="O68" s="14"/>
-      <c r="P68" s="21" t="s">
+      <c r="P68" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="Q68" s="21"/>
-      <c r="R68" s="21" t="s">
+      <c r="Q68" s="25"/>
+      <c r="R68" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="S68" s="21"/>
-      <c r="T68" s="21" t="s">
+      <c r="S68" s="25"/>
+      <c r="T68" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="U68" s="21"/>
+      <c r="U68" s="25"/>
       <c r="AB68" s="17"/>
       <c r="AC68" s="16"/>
     </row>
-    <row r="69" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B69" s="12">
         <v>67</v>
       </c>
@@ -1997,42 +2006,42 @@
       </c>
       <c r="N69" s="13"/>
       <c r="O69" s="14"/>
-      <c r="P69" s="21" t="s">
+      <c r="P69" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="Q69" s="21"/>
-      <c r="R69" s="21" t="s">
+      <c r="Q69" s="25"/>
+      <c r="R69" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="S69" s="21"/>
-      <c r="T69" s="21" t="s">
+      <c r="S69" s="25"/>
+      <c r="T69" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="U69" s="21"/>
+      <c r="U69" s="25"/>
       <c r="AB69" s="17"/>
       <c r="AC69" s="16"/>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B70">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B71">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B72">
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B73">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B74" s="12">
         <v>72</v>
       </c>
@@ -2055,7 +2064,7 @@
       <c r="AB74" s="6"/>
       <c r="AC74" s="16"/>
     </row>
-    <row r="75" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B75" s="12">
         <v>73</v>
       </c>
@@ -2072,7 +2081,7 @@
       <c r="AB75" s="17"/>
       <c r="AC75" s="16"/>
     </row>
-    <row r="76" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B76" s="12">
         <v>74</v>
       </c>
@@ -2089,7 +2098,7 @@
       <c r="AB76" s="17"/>
       <c r="AC76" s="16"/>
     </row>
-    <row r="77" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B77" s="12">
         <v>75</v>
       </c>
@@ -2106,102 +2115,102 @@
       <c r="AB77" s="17"/>
       <c r="AC77" s="16"/>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B78">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B79">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.4">
       <c r="B80">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B81">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B82">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B83">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B84">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B85">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B86">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B87">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B88">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B89">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B90">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B91">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B92">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B93">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B94">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B95">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B96">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>77</v>
       </c>
@@ -2240,7 +2249,7 @@
       </c>
       <c r="AB97" s="6"/>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B98">
         <v>96</v>
       </c>
@@ -2251,7 +2260,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B99">
         <v>97</v>
       </c>
@@ -2262,7 +2271,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B100">
         <v>98</v>
       </c>
@@ -2273,37 +2282,37 @@
         <v>29</v>
       </c>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B101">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B102">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B103">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B104">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B105">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B106">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B107">
         <v>105</v>
       </c>
@@ -2330,452 +2339,452 @@
       </c>
       <c r="AB107" s="6"/>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B108">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B109">
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B110">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B111">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:28" x14ac:dyDescent="0.4">
       <c r="B112">
         <v>110</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B113">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B114">
         <v>112</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B115">
         <v>113</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B116">
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B117">
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B118">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B119">
         <v>117</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B120">
         <v>118</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B121">
         <v>119</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B122">
         <v>120</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B123">
         <v>121</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B124">
         <v>122</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B125">
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B126">
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B127">
         <v>125</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B128">
         <v>126</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B129">
         <v>127</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B130">
         <v>128</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B131">
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B132">
         <v>130</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B133">
         <v>131</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B134">
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B135">
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B136">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B137">
         <v>135</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B138">
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B139">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B140">
         <v>138</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B141">
         <v>139</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B142">
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B143">
         <v>141</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B144">
         <v>142</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B145">
         <v>143</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B146">
         <v>144</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B147">
         <v>145</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B148">
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B149">
         <v>147</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B150">
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B151">
         <v>149</v>
       </c>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B152">
         <v>150</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B153">
         <v>151</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B154">
         <v>152</v>
       </c>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B155">
         <v>153</v>
       </c>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B156">
         <v>154</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B157">
         <v>155</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B158">
         <v>156</v>
       </c>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B159">
         <v>157</v>
       </c>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B160">
         <v>158</v>
       </c>
     </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B161">
         <v>159</v>
       </c>
     </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B162">
         <v>160</v>
       </c>
     </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B163">
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B164">
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B165">
         <v>163</v>
       </c>
     </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B166">
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B167">
         <v>165</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B168">
         <v>166</v>
       </c>
     </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B169">
         <v>167</v>
       </c>
     </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B170">
         <v>168</v>
       </c>
     </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B171">
         <v>169</v>
       </c>
     </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B172">
         <v>170</v>
       </c>
     </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B173">
         <v>171</v>
       </c>
     </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B174">
         <v>172</v>
       </c>
     </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B175">
         <v>173</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B176">
         <v>174</v>
       </c>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B177">
         <v>175</v>
       </c>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B178">
         <v>176</v>
       </c>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B179">
         <v>177</v>
       </c>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B180">
         <v>178</v>
       </c>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B181">
         <v>179</v>
       </c>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B182">
         <v>180</v>
       </c>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B183">
         <v>181</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B184">
         <v>182</v>
       </c>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B185">
         <v>183</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B186">
         <v>184</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B187">
         <v>185</v>
       </c>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B188">
         <v>186</v>
       </c>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B189">
         <v>187</v>
       </c>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B190">
         <v>188</v>
       </c>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B191">
         <v>189</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B192">
         <v>190</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B193">
         <v>191</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B194">
         <v>192</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B195">
         <v>193</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B196">
         <v>194</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A197" t="s">
         <v>78</v>
       </c>
@@ -2783,528 +2792,539 @@
         <v>195</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B198">
         <v>196</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B199">
         <v>197</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B200">
         <v>198</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B201">
         <v>199</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B202">
         <v>200</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B203">
         <v>201</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B204">
         <v>202</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B205">
         <v>203</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B206">
         <v>204</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B207">
         <v>205</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.4">
       <c r="B208">
         <v>206</v>
       </c>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B209">
         <v>207</v>
       </c>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B210">
         <v>208</v>
       </c>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B211">
         <v>209</v>
       </c>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B212">
         <v>210</v>
       </c>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B213">
         <v>211</v>
       </c>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B214">
         <v>212</v>
       </c>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B215">
         <v>213</v>
       </c>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B216">
         <v>214</v>
       </c>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B217">
         <v>215</v>
       </c>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B218">
         <v>216</v>
       </c>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B219">
         <v>217</v>
       </c>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B220">
         <v>218</v>
       </c>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B221">
         <v>219</v>
       </c>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B222">
         <v>220</v>
       </c>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B223">
         <v>221</v>
       </c>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B224">
         <v>222</v>
       </c>
     </row>
-    <row r="225" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B225">
         <v>223</v>
       </c>
     </row>
-    <row r="226" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B226">
         <v>224</v>
       </c>
     </row>
-    <row r="227" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B227">
         <v>225</v>
       </c>
     </row>
-    <row r="228" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B228">
         <v>226</v>
       </c>
     </row>
-    <row r="229" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B229">
         <v>227</v>
       </c>
     </row>
-    <row r="230" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B230">
         <v>228</v>
       </c>
     </row>
-    <row r="231" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B231">
         <v>229</v>
       </c>
     </row>
-    <row r="232" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B232">
         <v>230</v>
       </c>
     </row>
-    <row r="233" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B233">
         <v>231</v>
       </c>
     </row>
-    <row r="234" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B234">
         <v>232</v>
       </c>
     </row>
-    <row r="235" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B235">
         <v>233</v>
       </c>
     </row>
-    <row r="236" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B236">
         <v>234</v>
       </c>
     </row>
-    <row r="237" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B237">
         <v>235</v>
       </c>
     </row>
-    <row r="238" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B238">
         <v>236</v>
       </c>
     </row>
-    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B239">
         <v>237</v>
       </c>
     </row>
-    <row r="240" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B240">
         <v>238</v>
       </c>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B241">
         <v>239</v>
       </c>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B242">
         <v>240</v>
       </c>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B243">
         <v>241</v>
       </c>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B244">
         <v>242</v>
       </c>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B245">
         <v>243</v>
       </c>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B246">
         <v>244</v>
       </c>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B247">
         <v>245</v>
       </c>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B248">
         <v>246</v>
       </c>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B249">
         <v>247</v>
       </c>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B250">
         <v>248</v>
       </c>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B251">
         <v>249</v>
       </c>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B252">
         <v>250</v>
       </c>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B253">
         <v>251</v>
       </c>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B254">
         <v>252</v>
       </c>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B255">
         <v>253</v>
       </c>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B256">
         <v>254</v>
       </c>
     </row>
-    <row r="257" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B257">
         <v>255</v>
       </c>
     </row>
-    <row r="258" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B258">
         <v>256</v>
       </c>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B259">
         <v>257</v>
       </c>
     </row>
-    <row r="260" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B260">
         <v>258</v>
       </c>
     </row>
-    <row r="261" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B261">
         <v>259</v>
       </c>
     </row>
-    <row r="262" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B262">
         <v>260</v>
       </c>
     </row>
-    <row r="263" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B263">
         <v>261</v>
       </c>
     </row>
-    <row r="264" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B264">
         <v>262</v>
       </c>
     </row>
-    <row r="265" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B265">
         <v>263</v>
       </c>
     </row>
-    <row r="266" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B266">
         <v>264</v>
       </c>
     </row>
-    <row r="267" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B267">
         <v>265</v>
       </c>
     </row>
-    <row r="268" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B268">
         <v>266</v>
       </c>
     </row>
-    <row r="269" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B269">
         <v>267</v>
       </c>
     </row>
-    <row r="270" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B270">
         <v>268</v>
       </c>
     </row>
-    <row r="271" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B271">
         <v>269</v>
       </c>
     </row>
-    <row r="272" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B272">
         <v>270</v>
       </c>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B273">
         <v>271</v>
       </c>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="274" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B274">
         <v>272</v>
       </c>
     </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="275" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B275">
         <v>273</v>
       </c>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="276" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B276">
         <v>274</v>
       </c>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="277" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B277">
         <v>275</v>
       </c>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="278" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B278">
         <v>276</v>
       </c>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="279" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B279">
         <v>277</v>
       </c>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="280" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B280">
         <v>278</v>
       </c>
     </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="281" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B281">
         <v>279</v>
       </c>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="282" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B282">
         <v>280</v>
       </c>
     </row>
-    <row r="283" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B283">
         <v>281</v>
       </c>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="284" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B284">
         <v>282</v>
       </c>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B285">
         <v>283</v>
       </c>
     </row>
-    <row r="286" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="286" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B286">
         <v>284</v>
       </c>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="287" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B287">
         <v>285</v>
       </c>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="288" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B288">
         <v>286</v>
       </c>
     </row>
-    <row r="289" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="289" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B289">
         <v>287</v>
       </c>
     </row>
-    <row r="290" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="290" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B290">
         <v>288</v>
       </c>
     </row>
-    <row r="291" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="291" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B291">
         <v>289</v>
       </c>
     </row>
-    <row r="292" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="292" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B292">
         <v>290</v>
       </c>
     </row>
-    <row r="293" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="293" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B293">
         <v>291</v>
       </c>
     </row>
-    <row r="294" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="294" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B294">
         <v>292</v>
       </c>
     </row>
-    <row r="295" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="295" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B295">
         <v>293</v>
       </c>
     </row>
-    <row r="296" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="296" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B296">
         <v>294</v>
       </c>
     </row>
-    <row r="297" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="297" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B297">
         <v>295</v>
       </c>
     </row>
-    <row r="298" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="298" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B298">
         <v>296</v>
       </c>
     </row>
-    <row r="299" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="299" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B299">
         <v>297</v>
       </c>
     </row>
-    <row r="300" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="300" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B300">
         <v>298</v>
       </c>
     </row>
-    <row r="301" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="301" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B301">
         <v>299</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="P54:Q54"/>
+    <mergeCell ref="P55:Q55"/>
+    <mergeCell ref="P56:Q56"/>
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="P58:Q58"/>
+    <mergeCell ref="P68:Q68"/>
+    <mergeCell ref="P67:Q67"/>
     <mergeCell ref="R67:S67"/>
     <mergeCell ref="T67:U67"/>
     <mergeCell ref="P69:Q69"/>
@@ -3312,17 +3332,6 @@
     <mergeCell ref="T69:U69"/>
     <mergeCell ref="R68:S68"/>
     <mergeCell ref="T68:U68"/>
-    <mergeCell ref="P55:Q55"/>
-    <mergeCell ref="P56:Q56"/>
-    <mergeCell ref="P57:Q57"/>
-    <mergeCell ref="P58:Q58"/>
-    <mergeCell ref="P68:Q68"/>
-    <mergeCell ref="P67:Q67"/>
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="P54:Q54"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
@@ -3346,26 +3355,26 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="51.42578125" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.84375" customWidth="1"/>
+    <col min="3" max="3" width="51.3828125" customWidth="1"/>
+    <col min="4" max="4" width="48.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:7" ht="19.75" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="17.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -3379,7 +3388,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="105.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="102.45" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3393,7 +3402,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>100</v>
       </c>
@@ -3401,13 +3410,13 @@
         <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3421,7 +3430,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="72.900000000000006" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3429,13 +3438,13 @@
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="116.6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -3443,10 +3452,10 @@
         <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -3457,17 +3466,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -3475,7 +3484,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>89</v>
       </c>
@@ -3483,10 +3492,10 @@
         <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -3497,7 +3506,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -3508,7 +3517,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -3519,7 +3528,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -3530,7 +3539,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Include CANBus features for dashboard
-2 possible modes of operation:
1)define CAN_CONNECTED to enable CANBus features
2) undefine CAN_CONNECTED to use it without CANBus (i.e. for debug)
--CANBus untested

-Lighting characteristic not updated from the ESP anymore (only update through phone)
</commit_message>
<xml_diff>
--- a/arduino/CAN Bus/CAN Bus Messages.xlsx
+++ b/arduino/CAN Bus/CAN Bus Messages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/CAN Bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="769" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC067EEC-56DB-4D73-B2D4-1B5855CED67B}"/>
+  <xr:revisionPtr revIDLastSave="808" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F78317DD-3026-4F04-828C-8B910DEAB7A5}"/>
   <bookViews>
-    <workbookView xWindow="22425" yWindow="9120" windowWidth="22875" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2880" yWindow="1950" windowWidth="22875" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="174">
   <si>
     <t>Message ID (Decimal)</t>
   </si>
@@ -356,15 +356,9 @@
     <t>RR</t>
   </si>
   <si>
-    <t>Wheel speed (RPM) = (B1*256 + B2)*0.03; 0-1966RPM</t>
-  </si>
-  <si>
     <t>same</t>
   </si>
   <si>
-    <t>Speed (km/h) = (B1*56 + B2)/256; 0-256km/h</t>
-  </si>
-  <si>
     <t>R value</t>
   </si>
   <si>
@@ -372,9 +366,6 @@
   </si>
   <si>
     <t>B value</t>
-  </si>
-  <si>
-    <t>fade/chase (to be developed)</t>
   </si>
   <si>
     <t xml:space="preserve">indicator on </t>
@@ -482,9 +473,6 @@
     <t>0 =  error, 1 = ok, 255 = offline</t>
   </si>
   <si>
-    <t>brake 0( off) or 1 (on)</t>
-  </si>
-  <si>
     <t>FW</t>
   </si>
   <si>
@@ -558,6 +546,30 @@
   </si>
   <si>
     <t>brake percent (%); 0-100%. Could be calculated based on pressure</t>
+  </si>
+  <si>
+    <t>Wheel speed (RPM) = (B1*256 + B0)*0.03; 0-1966RPM</t>
+  </si>
+  <si>
+    <t>Speed (km/h) = (B1*256 + B0)/256; 0-256km/h</t>
+  </si>
+  <si>
+    <t>reverse (0: forward, 1: reverse)</t>
+  </si>
+  <si>
+    <t>IMU Status</t>
+  </si>
+  <si>
+    <t>FL Status</t>
+  </si>
+  <si>
+    <t>RL Status</t>
+  </si>
+  <si>
+    <t>INT Status</t>
+  </si>
+  <si>
+    <t>fade (0: fade, 1: immediately change)</t>
   </si>
 </sst>
 </file>
@@ -1051,10 +1063,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="V38" sqref="V38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,7 +1108,7 @@
       </c>
       <c r="O1" s="10"/>
       <c r="P1" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>84</v>
@@ -1176,7 +1188,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>51</v>
@@ -1191,7 +1203,7 @@
         <v>58</v>
       </c>
       <c r="P6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="AB6" s="6" t="s">
         <v>53</v>
@@ -1234,14 +1246,14 @@
         <v>22</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AB10" s="22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="AC10" s="23"/>
     </row>
@@ -1262,11 +1274,11 @@
         <v>22</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="O11" s="21"/>
       <c r="P11" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AB11" s="24"/>
       <c r="AC11" s="23"/>
@@ -1276,7 +1288,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>82</v>
@@ -1288,11 +1300,11 @@
         <v>22</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="O12" s="21"/>
       <c r="P12" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AB12" s="24"/>
       <c r="AC12" s="23"/>
@@ -1314,11 +1326,11 @@
         <v>22</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="O13" s="21"/>
       <c r="P13" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="AB13" s="24"/>
       <c r="AC13" s="23"/>
@@ -1328,76 +1340,140 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>160</v>
+        <v>169</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="M14" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>163</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="O14" s="21"/>
       <c r="P14" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>13</v>
       </c>
+      <c r="C15" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="P15" s="19" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>14</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="M16" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="N16" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="P16" s="19" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>4</v>
       </c>
       <c r="M17" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>16</v>
       </c>
+      <c r="C18" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="M18" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="P18" s="19" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>17</v>
       </c>
+      <c r="C19" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="M19" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="P19" s="19" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>18</v>
       </c>
+      <c r="C20" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="M20" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="P20" s="19" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>19</v>
       </c>
+      <c r="C21" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="M21" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="P21" s="19" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22">
@@ -1485,13 +1561,13 @@
         <v>63</v>
       </c>
       <c r="P34" t="s">
+        <v>161</v>
+      </c>
+      <c r="R34" t="s">
+        <v>162</v>
+      </c>
+      <c r="T34" t="s">
         <v>165</v>
-      </c>
-      <c r="R34" t="s">
-        <v>166</v>
-      </c>
-      <c r="T34" t="s">
-        <v>169</v>
       </c>
       <c r="Y34">
         <v>51</v>
@@ -1568,11 +1644,11 @@
         <v>59</v>
       </c>
       <c r="P38" s="26" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="Q38" s="26"/>
       <c r="R38" s="26" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="S38" s="26"/>
       <c r="T38" s="26" t="s">
@@ -1644,7 +1720,7 @@
         <v>63</v>
       </c>
       <c r="P46" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="R46" t="s">
         <v>101</v>
@@ -1671,7 +1747,7 @@
         <v>48</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>4</v>
@@ -1704,10 +1780,10 @@
         <v>105</v>
       </c>
       <c r="T50" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="U50" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1790,9 +1866,12 @@
         <v>63</v>
       </c>
       <c r="P54" s="26" t="s">
-        <v>106</v>
+        <v>166</v>
       </c>
       <c r="Q54" s="26"/>
+      <c r="R54" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="55" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B55">
@@ -1808,9 +1887,12 @@
         <v>4</v>
       </c>
       <c r="P55" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q55" s="26"/>
+      <c r="R55" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="56" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B56">
@@ -1826,9 +1908,12 @@
         <v>4</v>
       </c>
       <c r="P56" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q56" s="26"/>
+      <c r="R56" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="57" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B57">
@@ -1844,9 +1929,12 @@
         <v>4</v>
       </c>
       <c r="P57" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q57" s="26"/>
+      <c r="R57" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="58" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B58">
@@ -1865,9 +1953,12 @@
         <v>59</v>
       </c>
       <c r="P58" s="26" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="Q58" s="26"/>
+      <c r="R58" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="59" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B59">
@@ -1922,25 +2013,25 @@
       </c>
       <c r="O66" s="14"/>
       <c r="P66" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Q66" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="R66" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="S66" s="12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="T66" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="U66" s="12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AB66" s="15" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="AC66" s="16"/>
     </row>
@@ -1949,7 +2040,7 @@
         <v>65</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D67" s="13" t="s">
         <v>71</v>
@@ -1957,19 +2048,19 @@
       <c r="N67" s="13"/>
       <c r="O67" s="14"/>
       <c r="P67" s="25" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Q67" s="25"/>
       <c r="R67" s="25" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="S67" s="25"/>
       <c r="T67" s="25" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="U67" s="25"/>
       <c r="AB67" s="17" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="AC67" s="16"/>
     </row>
@@ -1978,7 +2069,7 @@
         <v>66</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D68" s="13" t="s">
         <v>71</v>
@@ -1986,15 +2077,15 @@
       <c r="N68" s="13"/>
       <c r="O68" s="14"/>
       <c r="P68" s="25" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="Q68" s="25"/>
       <c r="R68" s="25" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="S68" s="25"/>
       <c r="T68" s="25" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="U68" s="25"/>
       <c r="AB68" s="17"/>
@@ -2005,7 +2096,7 @@
         <v>67</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D69" s="13" t="s">
         <v>71</v>
@@ -2013,15 +2104,15 @@
       <c r="N69" s="13"/>
       <c r="O69" s="14"/>
       <c r="P69" s="25" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="Q69" s="25"/>
       <c r="R69" s="25" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="S69" s="25"/>
       <c r="T69" s="25" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="U69" s="25"/>
       <c r="AB69" s="17"/>
@@ -2062,10 +2153,10 @@
       </c>
       <c r="O74" s="14"/>
       <c r="P74" s="12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Q74" s="12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AB74" s="6"/>
       <c r="AC74" s="16"/>
@@ -2230,34 +2321,31 @@
         <v>96</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E98" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="N98" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="N98" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="P98" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>108</v>
+      </c>
+      <c r="R98" t="s">
         <v>109</v>
       </c>
-      <c r="Q98" t="s">
+      <c r="S98" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="T98" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="R98" t="s">
-        <v>111</v>
-      </c>
-      <c r="S98" t="s">
-        <v>144</v>
-      </c>
-      <c r="T98" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="U98" s="12" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.25">
@@ -2265,7 +2353,7 @@
         <v>97</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>22</v>
@@ -2274,31 +2362,29 @@
         <v>104</v>
       </c>
       <c r="N99" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="P99" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q99" t="s">
+        <v>108</v>
+      </c>
+      <c r="R99" t="s">
         <v>109</v>
       </c>
-      <c r="Q99" t="s">
+      <c r="S99" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="T99" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="R99" t="s">
-        <v>111</v>
-      </c>
-      <c r="S99" t="s">
-        <v>144</v>
-      </c>
-      <c r="T99" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="U99" s="12" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="100" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>98</v>
       </c>
+      <c r="S100" s="19"/>
     </row>
     <row r="101" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B101">
@@ -2314,16 +2400,19 @@
         <v>13</v>
       </c>
       <c r="N101" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="P101" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>108</v>
+      </c>
+      <c r="R101" t="s">
         <v>109</v>
       </c>
-      <c r="Q101" t="s">
-        <v>110</v>
-      </c>
-      <c r="R101" t="s">
-        <v>111</v>
+      <c r="S101" s="19" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.25">
@@ -3400,7 +3489,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -3428,7 +3517,7 @@
         <v>83</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D4" t="s">
         <v>67</v>
@@ -3456,7 +3545,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D6" t="s">
         <v>38</v>
@@ -3470,24 +3559,24 @@
         <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3495,7 +3584,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3514,15 +3603,15 @@
         <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>36</v>
@@ -3533,13 +3622,13 @@
         <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3550,7 +3639,7 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Front Wheels node code for arduino
</commit_message>
<xml_diff>
--- a/arduino/CAN Bus/CAN Bus Messages.xlsx
+++ b/arduino/CAN Bus/CAN Bus Messages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sutdapac-my.sharepoint.com/personal/nigel_gomes_mymail_sutd_edu_sg/Documents/Documents/GitHub/evam-dashboard/arduino/CAN Bus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="808" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F78317DD-3026-4F04-828C-8B910DEAB7A5}"/>
+  <xr:revisionPtr revIDLastSave="815" documentId="11_F25DC773A252ABDACC104822919F401C5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7CE6A63-C758-4315-BC83-1D984DD9678A}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="1950" windowWidth="22875" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15525" yWindow="5130" windowWidth="22875" windowHeight="16470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="172">
   <si>
     <t>Message ID (Decimal)</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>&lt;reserved&gt;</t>
-  </si>
-  <si>
-    <t>HUD or ECU</t>
   </si>
   <si>
     <t>HUD(?)</t>
@@ -426,9 +423,6 @@
   </si>
   <si>
     <t>(Damper?) Linear travel</t>
-  </si>
-  <si>
-    <t>angle = (B1*256 + B2)/10 - 180; 0-360</t>
   </si>
   <si>
     <t>for ECU and HUD to know that they are still connected</t>
@@ -512,9 +506,6 @@
     <t>Long Description / Functions</t>
   </si>
   <si>
-    <t>Reverse: 0: forward; 255: reverse</t>
-  </si>
-  <si>
     <t>Boost: 0: normal 255: boost</t>
   </si>
   <si>
@@ -570,6 +561,9 @@
   </si>
   <si>
     <t>fade (0: fade, 1: immediately change)</t>
+  </si>
+  <si>
+    <t>angle = (B1*256 + B0)/10 - 180; 0-360</t>
   </si>
 </sst>
 </file>
@@ -752,13 +746,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1063,10 +1057,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="V38" sqref="V38"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,50 +1086,50 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
       <c r="N1" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O1" s="10"/>
       <c r="P1" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="AB1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AC1" s="7"/>
       <c r="AD1" s="1" t="s">
@@ -1144,7 +1138,7 @@
     </row>
     <row r="2" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1188,25 +1182,25 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
       <c r="M6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="P6" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB6" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="P6" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB6" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1246,14 +1240,14 @@
         <v>22</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O10" s="21"/>
       <c r="P10" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AB10" s="22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AC10" s="23"/>
     </row>
@@ -1274,11 +1268,11 @@
         <v>22</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O11" s="21"/>
       <c r="P11" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AB11" s="24"/>
       <c r="AC11" s="23"/>
@@ -1288,10 +1282,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>4</v>
@@ -1300,11 +1294,11 @@
         <v>22</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O12" s="21"/>
       <c r="P12" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AB12" s="24"/>
       <c r="AC12" s="23"/>
@@ -1326,11 +1320,11 @@
         <v>22</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O13" s="21"/>
       <c r="P13" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AB13" s="24"/>
       <c r="AC13" s="23"/>
@@ -1340,20 +1334,20 @@
         <v>12</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M14" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="O14" s="21"/>
       <c r="P14" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
@@ -1361,10 +1355,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>4</v>
@@ -1373,10 +1367,10 @@
         <v>22</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -1389,7 +1383,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>4</v>
@@ -1398,10 +1392,10 @@
         <v>22</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
@@ -1409,7 +1403,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E18" s="19" t="s">
         <v>4</v>
@@ -1418,10 +1412,10 @@
         <v>22</v>
       </c>
       <c r="N18" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -1429,16 +1423,16 @@
         <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="M19" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N19" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
@@ -1446,16 +1440,16 @@
         <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="M20" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
@@ -1463,16 +1457,16 @@
         <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="M21" s="19" t="s">
         <v>22</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -1540,16 +1534,16 @@
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34">
         <v>32</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E34" t="s">
         <v>4</v>
@@ -1558,16 +1552,16 @@
         <v>22</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P34" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="R34" t="s">
+        <v>159</v>
+      </c>
+      <c r="T34" t="s">
         <v>162</v>
-      </c>
-      <c r="T34" t="s">
-        <v>165</v>
       </c>
       <c r="Y34">
         <v>51</v>
@@ -1582,7 +1576,7 @@
         <v>30</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>4</v>
@@ -1597,17 +1591,17 @@
         <v>22</v>
       </c>
       <c r="N35" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O35" s="14"/>
       <c r="P35" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Y35" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AB35" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AC35" s="16"/>
     </row>
@@ -1629,37 +1623,37 @@
         <v>36</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M38" t="s">
         <v>22</v>
       </c>
       <c r="N38" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P38" s="26" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Q38" s="26"/>
       <c r="R38" s="26" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="S38" s="26"/>
       <c r="T38" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U38" s="26"/>
       <c r="V38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="W38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AB38" s="6"/>
     </row>
@@ -1714,16 +1708,16 @@
         <v>4</v>
       </c>
       <c r="M46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N46" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P46" t="s">
-        <v>130</v>
+        <v>171</v>
       </c>
       <c r="R46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AB46" s="6"/>
     </row>
@@ -1747,7 +1741,7 @@
         <v>48</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>4</v>
@@ -1765,25 +1759,25 @@
         <v>20</v>
       </c>
       <c r="N50" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P50" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q50" t="s">
         <v>102</v>
       </c>
-      <c r="Q50" t="s">
+      <c r="R50" t="s">
         <v>103</v>
       </c>
-      <c r="R50" t="s">
+      <c r="S50" t="s">
         <v>104</v>
       </c>
-      <c r="S50" t="s">
-        <v>105</v>
-      </c>
       <c r="T50" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="U50" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="2:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1802,7 +1796,7 @@
       <c r="N51" s="13"/>
       <c r="O51" s="14"/>
       <c r="P51" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AB51" s="17"/>
       <c r="AC51" s="16"/>
@@ -1823,7 +1817,7 @@
       <c r="N52" s="13"/>
       <c r="O52" s="14"/>
       <c r="P52" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AB52" s="17"/>
       <c r="AC52" s="16"/>
@@ -1844,7 +1838,7 @@
       <c r="N53" s="13"/>
       <c r="O53" s="14"/>
       <c r="P53" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AB53" s="17"/>
       <c r="AC53" s="16"/>
@@ -1863,14 +1857,14 @@
         <v>4</v>
       </c>
       <c r="N54" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P54" s="26" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="Q54" s="26"/>
       <c r="R54" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="2:29" x14ac:dyDescent="0.25">
@@ -1887,11 +1881,11 @@
         <v>4</v>
       </c>
       <c r="P55" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q55" s="26"/>
       <c r="R55" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="2:29" x14ac:dyDescent="0.25">
@@ -1908,11 +1902,11 @@
         <v>4</v>
       </c>
       <c r="P56" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q56" s="26"/>
       <c r="R56" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="57" spans="2:29" x14ac:dyDescent="0.25">
@@ -1929,11 +1923,11 @@
         <v>4</v>
       </c>
       <c r="P57" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q57" s="26"/>
       <c r="R57" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="2:29" x14ac:dyDescent="0.25">
@@ -1941,7 +1935,7 @@
         <v>56</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>4</v>
@@ -1950,14 +1944,14 @@
         <v>22</v>
       </c>
       <c r="N58" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P58" s="26" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="Q58" s="26"/>
       <c r="R58" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" spans="2:29" x14ac:dyDescent="0.25">
@@ -1997,41 +1991,41 @@
     </row>
     <row r="66" spans="1:29" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B66" s="12">
         <v>64</v>
       </c>
       <c r="C66" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="N66" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="D66" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="N66" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="O66" s="14"/>
       <c r="P66" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q66" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="Q66" s="12" t="s">
+      <c r="R66" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="R66" s="12" t="s">
-        <v>116</v>
-      </c>
       <c r="S66" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="T66" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="T66" s="12" t="s">
+      <c r="U66" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="U66" s="12" t="s">
-        <v>113</v>
-      </c>
       <c r="AB66" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AC66" s="16"/>
     </row>
@@ -2040,27 +2034,27 @@
         <v>65</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N67" s="13"/>
       <c r="O67" s="14"/>
-      <c r="P67" s="25" t="s">
+      <c r="P67" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q67" s="27"/>
+      <c r="R67" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="Q67" s="25"/>
-      <c r="R67" s="25" t="s">
+      <c r="S67" s="27"/>
+      <c r="T67" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="S67" s="25"/>
-      <c r="T67" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="U67" s="25"/>
+      <c r="U67" s="27"/>
       <c r="AB67" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AC67" s="16"/>
     </row>
@@ -2069,25 +2063,25 @@
         <v>66</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D68" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N68" s="13"/>
       <c r="O68" s="14"/>
-      <c r="P68" s="25" t="s">
+      <c r="P68" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q68" s="27"/>
+      <c r="R68" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="Q68" s="25"/>
-      <c r="R68" s="25" t="s">
+      <c r="S68" s="27"/>
+      <c r="T68" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="S68" s="25"/>
-      <c r="T68" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="U68" s="25"/>
+      <c r="U68" s="27"/>
       <c r="AB68" s="17"/>
       <c r="AC68" s="16"/>
     </row>
@@ -2096,25 +2090,25 @@
         <v>67</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N69" s="13"/>
       <c r="O69" s="14"/>
-      <c r="P69" s="25" t="s">
+      <c r="P69" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q69" s="27"/>
+      <c r="R69" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="Q69" s="25"/>
-      <c r="R69" s="25" t="s">
+      <c r="S69" s="27"/>
+      <c r="T69" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="S69" s="25"/>
-      <c r="T69" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="U69" s="25"/>
+      <c r="U69" s="27"/>
       <c r="AB69" s="17"/>
       <c r="AC69" s="16"/>
     </row>
@@ -2143,20 +2137,20 @@
         <v>72</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N74" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O74" s="14"/>
       <c r="P74" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Q74" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AB74" s="6"/>
       <c r="AC74" s="16"/>
@@ -2166,13 +2160,13 @@
         <v>73</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N75" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O75" s="14"/>
       <c r="AB75" s="17"/>
@@ -2183,13 +2177,13 @@
         <v>74</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N76" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O76" s="14"/>
       <c r="AB76" s="17"/>
@@ -2200,13 +2194,13 @@
         <v>75</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N77" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O77" s="14"/>
       <c r="AB77" s="17"/>
@@ -2315,37 +2309,37 @@
     </row>
     <row r="98" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B98">
         <v>96</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E98" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="N98" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P98" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q98" t="s">
         <v>107</v>
       </c>
-      <c r="Q98" t="s">
+      <c r="R98" t="s">
         <v>108</v>
       </c>
-      <c r="R98" t="s">
+      <c r="S98" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="T98" s="12" t="s">
         <v>109</v>
-      </c>
-      <c r="S98" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="T98" s="12" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="99" spans="1:28" x14ac:dyDescent="0.25">
@@ -2353,31 +2347,31 @@
         <v>97</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E99" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N99" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P99" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q99" t="s">
         <v>107</v>
       </c>
-      <c r="Q99" t="s">
+      <c r="R99" t="s">
         <v>108</v>
       </c>
-      <c r="R99" t="s">
+      <c r="S99" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="T99" s="12" t="s">
         <v>109</v>
-      </c>
-      <c r="S99" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="T99" s="12" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="100" spans="1:28" x14ac:dyDescent="0.25">
@@ -2400,19 +2394,19 @@
         <v>13</v>
       </c>
       <c r="N101" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P101" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q101" t="s">
         <v>107</v>
       </c>
-      <c r="Q101" t="s">
+      <c r="R101" t="s">
         <v>108</v>
       </c>
-      <c r="R101" t="s">
-        <v>109</v>
-      </c>
       <c r="S101" s="19" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="102" spans="1:28" x14ac:dyDescent="0.25">
@@ -2893,7 +2887,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B197">
         <v>195</v>
@@ -3421,17 +3415,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E1:M1"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="R38:S38"/>
-    <mergeCell ref="T38:U38"/>
-    <mergeCell ref="P54:Q54"/>
-    <mergeCell ref="P55:Q55"/>
-    <mergeCell ref="P56:Q56"/>
-    <mergeCell ref="P57:Q57"/>
-    <mergeCell ref="P58:Q58"/>
-    <mergeCell ref="P68:Q68"/>
-    <mergeCell ref="P67:Q67"/>
     <mergeCell ref="R67:S67"/>
     <mergeCell ref="T67:U67"/>
     <mergeCell ref="P69:Q69"/>
@@ -3439,6 +3422,17 @@
     <mergeCell ref="T69:U69"/>
     <mergeCell ref="R68:S68"/>
     <mergeCell ref="T68:U68"/>
+    <mergeCell ref="P55:Q55"/>
+    <mergeCell ref="P56:Q56"/>
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="P58:Q58"/>
+    <mergeCell ref="P68:Q68"/>
+    <mergeCell ref="P67:Q67"/>
+    <mergeCell ref="E1:M1"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="R38:S38"/>
+    <mergeCell ref="T38:U38"/>
+    <mergeCell ref="P54:Q54"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
@@ -3489,7 +3483,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -3506,21 +3500,21 @@
         <v>26</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
         <v>82</v>
       </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3534,7 +3528,7 @@
         <v>45</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3545,7 +3539,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D6" t="s">
         <v>38</v>
@@ -3559,24 +3553,24 @@
         <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3584,7 +3578,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3597,21 +3591,21 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
         <v>71</v>
       </c>
-      <c r="B15" t="s">
-        <v>72</v>
-      </c>
       <c r="C15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>36</v>
@@ -3619,16 +3613,16 @@
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3639,7 +3633,7 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>